<commit_message>
carga de usuarios demo 1
</commit_message>
<xml_diff>
--- a/Formatos/Formato Carga de Usuarios.xlsx
+++ b/Formatos/Formato Carga de Usuarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TESI Indicadores\Website Angular\Tesi-Indicadores-FrontEnd\src\assets\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TESI Indicadores\Website Angular\Tesi-Indicadores-FrontEnd\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1DD129-B08F-4F26-A57D-C2241D8D6676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284BBC6A-278E-4EF1-868D-3D3E43126DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E186D6C7-C6D6-47B6-9AF2-264C7F877308}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Formato" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Formato!$A$1:$G$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Formato!$A$1:$G$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Carrera</t>
   </si>
   <si>
-    <t>Formato para la Carga de Usuarios.                                                           (Nota no Modificar los nombres de las columnas)</t>
-  </si>
-  <si>
     <t>Mario Alberto</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
     <t>Administrador</t>
   </si>
   <si>
+    <t>ISC</t>
+  </si>
+  <si>
     <t>Ari Argenis</t>
   </si>
   <si>
@@ -74,15 +74,12 @@
   <si>
     <t>ari@tesi.org</t>
   </si>
-  <si>
-    <t>ISC</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,8 +102,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -115,14 +113,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -162,33 +152,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -215,13 +194,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -258,13 +237,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -301,13 +280,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -344,13 +323,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -387,13 +366,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -430,13 +409,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -473,13 +452,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -516,13 +495,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -559,13 +538,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -602,13 +581,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -645,13 +624,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -688,13 +667,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -731,13 +710,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -772,50 +751,61 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1428749</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2505074</xdr:colOff>
+      <xdr:colOff>2495551</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>739830</xdr:rowOff>
+      <xdr:rowOff>742950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Imagen 15">
+        <xdr:cNvPr id="17" name="Imagen 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{781A3794-159C-4A0B-8909-21D14BF1B74A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5D25602-855A-44DA-8A07-C0E7244E5A64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8934449" y="0"/>
-          <a:ext cx="1076325" cy="739830"/>
+          <a:off x="1" y="0"/>
+          <a:ext cx="10001250" cy="742950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1120,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9229E7-13F4-4225-BBED-27D055220375}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1138,96 +1128,88 @@
     <col min="8" max="1018" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="58.5" customHeight="1">
+    <row r="1" spans="1:7" ht="73.5" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="4">
-        <v>123456</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="9">
-        <v>123456</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="G7" s="8"/>
+    <row r="11" spans="1:7">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{41370590-E472-4772-BDD7-9DFCAB7B8138}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{28EC83DD-9B7B-4BDB-87DE-DB2982D2A6D2}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A1893ACD-8F5F-457D-8568-2F15FA83893B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{9014CC17-DB88-440A-A2D6-2CC229B71010}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup scale="58" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1246,6 +1228,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E2DB502ABF570459D92EAB368475EB9" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc33ec95a03d3916ee7c550885e77c05">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aa9ecf5a-f88a-4c81-95fd-fe1157aac7ad" xmlns:ns4="112e49ae-75ca-444f-98be-3b3ec7e22459" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9408b6cd564dfbdec8defa50352aa754" ns3:_="" ns4:_="">
     <xsd:import namespace="aa9ecf5a-f88a-4c81-95fd-fe1157aac7ad"/>
@@ -1416,12 +1404,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60FEB2BC-FDC5-4E40-9D1B-465E85B3F859}">
   <ds:schemaRefs>
@@ -1431,6 +1413,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC51C9C-65B9-47FB-87B3-21CF863618C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="112e49ae-75ca-444f-98be-3b3ec7e22459"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="aa9ecf5a-f88a-4c81-95fd-fe1157aac7ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D91726C-1B1F-487D-8645-98B7DB2DCA99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1447,21 +1446,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FC51C9C-65B9-47FB-87B3-21CF863618C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="112e49ae-75ca-444f-98be-3b3ec7e22459"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="aa9ecf5a-f88a-4c81-95fd-fe1157aac7ad"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>